<commit_message>
add all defect and fault in gui + test
</commit_message>
<xml_diff>
--- a/f2-02-04-5.xlsx
+++ b/f2-02-04-5.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="615" windowWidth="10215" windowHeight="11190"/>
+    <workbookView activeTab="0" windowHeight="11190" windowWidth="10215" xWindow="480" yWindow="615"/>
   </bookViews>
   <sheets>
-    <sheet name="1" sheetId="1" r:id="rId1"/>
+    <sheet name="1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="47">
   <si>
     <t>ПОВІДОМЛЕННЯ ПРО ДЕФЕКТИ</t>
   </si>
@@ -22,13 +22,13 @@
     <t>дата:</t>
   </si>
   <si>
-    <t>11/01/2018</t>
+    <t>15/01/2018</t>
   </si>
   <si>
     <t>час:</t>
   </si>
   <si>
-    <t>21:57</t>
+    <t>14:40</t>
   </si>
   <si>
     <t>Автор повідомлення:</t>
@@ -82,10 +82,10 @@
     <t>Рекваліфікація / EMPB</t>
   </si>
   <si>
+    <t>X</t>
+  </si>
+  <si>
     <t>Обладнання не вмикається / не продукує виріб</t>
-  </si>
-  <si>
-    <t>X</t>
   </si>
   <si>
     <t>Інше:</t>
@@ -161,66 +161,67 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="7">
     <font>
+      <name val="Calibri"/>
+      <charset val="204"/>
+      <family val="2"/>
+      <color theme="1"/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="Arial"/>
+      <charset val="238"/>
+      <family val="2"/>
+      <color theme="1"/>
       <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="238"/>
     </font>
     <font>
-      <b/>
+      <name val="Arial"/>
+      <charset val="238"/>
+      <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
       <sz val="16"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="238"/>
     </font>
     <font>
+      <name val="Arial"/>
+      <charset val="238"/>
+      <family val="2"/>
+      <color theme="1"/>
       <sz val="9"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="238"/>
     </font>
     <font>
-      <b/>
+      <name val="Calibri"/>
+      <charset val="238"/>
+      <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="Arial"/>
+      <charset val="238"/>
+      <family val="2"/>
+      <color rgb="FF000000"/>
       <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="238"/>
     </font>
     <font>
-      <b/>
+      <name val="Calibri"/>
+      <charset val="204"/>
+      <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -547,138 +548,137 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="57">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="3" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="4" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="5" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="7" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="8" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="9" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="10" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf borderId="6" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf borderId="11" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="12" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="13" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="14" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="15" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="9" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="4" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="11" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="17" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="18" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="19" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="20" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="21" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="21" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="22" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="18" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="21" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="16" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="23" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="24" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="25" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="26" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="27" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="28" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="29" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="16" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="9" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="4" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="11" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Обычный" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
 </file>
 
@@ -966,791 +966,794 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A3:N56"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A3:M56"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleSheetLayoutView="115" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0" zoomScaleSheetLayoutView="115">
       <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="1.140625" style="54" customWidth="1"/>
-    <col min="2" max="2" width="4.140625" style="54" customWidth="1"/>
-    <col min="7" max="7" width="3.5703125" style="54" customWidth="1"/>
-    <col min="8" max="8" width="4.140625" style="54" customWidth="1"/>
-    <col min="11" max="11" width="14.85546875" style="54" customWidth="1"/>
-    <col min="12" max="12" width="8.140625" style="54" customWidth="1"/>
-    <col min="13" max="13" width="1.85546875" style="54" customWidth="1"/>
-    <col min="14" max="14" width="2.28515625" style="54" customWidth="1"/>
+    <col customWidth="1" max="1" min="1" style="56" width="1.140625"/>
+    <col customWidth="1" max="2" min="2" style="56" width="4.140625"/>
+    <col customWidth="1" max="7" min="7" style="56" width="3.5703125"/>
+    <col customWidth="1" max="8" min="8" style="56" width="4.140625"/>
+    <col customWidth="1" max="11" min="11" style="56" width="14.85546875"/>
+    <col customWidth="1" max="12" min="12" style="56" width="8.140625"/>
+    <col customWidth="1" max="13" min="13" style="56" width="1.85546875"/>
+    <col customWidth="1" max="14" min="14" style="56" width="2.28515625"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:13" ht="20.25" customHeight="1">
+    <row customHeight="1" ht="20.25" r="3" s="56" spans="1:13">
       <c r="F3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="15.75" customHeight="1" thickBot="1"/>
-    <row r="6" spans="1:13" ht="3.95" customHeight="1">
-      <c r="A6" s="3"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="5"/>
+    <row customHeight="1" ht="15.75" r="5" s="56" spans="1:13" thickBot="1"/>
+    <row customHeight="1" ht="3.95" r="6" s="56" spans="1:13">
+      <c r="A6" s="3" t="n"/>
+      <c r="B6" s="4" t="n"/>
+      <c r="C6" s="4" t="n"/>
+      <c r="D6" s="4" t="n"/>
+      <c r="E6" s="4" t="n"/>
+      <c r="F6" s="4" t="n"/>
+      <c r="G6" s="4" t="n"/>
+      <c r="H6" s="4" t="n"/>
+      <c r="I6" s="4" t="n"/>
+      <c r="J6" s="4" t="n"/>
+      <c r="K6" s="4" t="n"/>
+      <c r="L6" s="4" t="n"/>
+      <c r="M6" s="5" t="n"/>
     </row>
     <row r="7" spans="1:13">
       <c r="A7" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="B7" s="10"/>
+      <c r="B7" s="10" t="n"/>
       <c r="C7" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="D7" s="16"/>
+      <c r="D7" s="16" t="n"/>
       <c r="E7" s="10" t="s">
         <v>3</v>
       </c>
       <c r="F7" s="44" t="s">
         <v>4</v>
       </c>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="10"/>
+      <c r="G7" s="12" t="n"/>
+      <c r="H7" s="12" t="n"/>
+      <c r="I7" s="10" t="n"/>
       <c r="J7" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="K7" s="44">
+      <c r="K7" s="44" t="n">
         <v>3012</v>
       </c>
-      <c r="L7" s="12"/>
-      <c r="M7" s="6"/>
-    </row>
-    <row r="8" spans="1:13" ht="3.95" customHeight="1" thickBot="1">
-      <c r="A8" s="7"/>
-      <c r="B8" s="22"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="22"/>
-      <c r="I8" s="22"/>
-      <c r="J8" s="22"/>
-      <c r="K8" s="22"/>
-      <c r="L8" s="22"/>
-      <c r="M8" s="9"/>
-    </row>
-    <row r="9" spans="1:13" ht="3.95" customHeight="1">
-      <c r="A9" s="3"/>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="23"/>
-      <c r="L9" s="23"/>
-      <c r="M9" s="5"/>
-    </row>
-    <row r="10" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A10" s="11"/>
+      <c r="L7" s="12" t="n"/>
+      <c r="M7" s="6" t="n"/>
+    </row>
+    <row customHeight="1" ht="3.95" r="8" s="56" spans="1:13" thickBot="1">
+      <c r="A8" s="7" t="n"/>
+      <c r="B8" s="22" t="n"/>
+      <c r="C8" s="22" t="n"/>
+      <c r="D8" s="22" t="n"/>
+      <c r="E8" s="22" t="n"/>
+      <c r="F8" s="22" t="n"/>
+      <c r="G8" s="22" t="n"/>
+      <c r="H8" s="22" t="n"/>
+      <c r="I8" s="22" t="n"/>
+      <c r="J8" s="22" t="n"/>
+      <c r="K8" s="22" t="n"/>
+      <c r="L8" s="22" t="n"/>
+      <c r="M8" s="9" t="n"/>
+    </row>
+    <row customHeight="1" ht="3.95" r="9" s="56" spans="1:13">
+      <c r="A9" s="3" t="n"/>
+      <c r="B9" s="23" t="n"/>
+      <c r="C9" s="23" t="n"/>
+      <c r="D9" s="23" t="n"/>
+      <c r="E9" s="23" t="n"/>
+      <c r="F9" s="23" t="n"/>
+      <c r="G9" s="23" t="n"/>
+      <c r="H9" s="23" t="n"/>
+      <c r="I9" s="23" t="n"/>
+      <c r="J9" s="23" t="n"/>
+      <c r="K9" s="23" t="n"/>
+      <c r="L9" s="23" t="n"/>
+      <c r="M9" s="5" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="10" s="56" spans="1:13" thickBot="1">
+      <c r="A10" s="11" t="n"/>
       <c r="C10" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="6"/>
-    </row>
-    <row r="11" spans="1:13" ht="15" customHeight="1" thickBot="1">
-      <c r="A11" s="11"/>
-      <c r="B11" s="47"/>
+      <c r="D10" s="12" t="n"/>
+      <c r="E10" s="12" t="n"/>
+      <c r="F10" s="12" t="n"/>
+      <c r="G10" s="12" t="n"/>
+      <c r="H10" s="12" t="n"/>
+      <c r="I10" s="12" t="n"/>
+      <c r="J10" s="12" t="n"/>
+      <c r="K10" s="12" t="n"/>
+      <c r="L10" s="12" t="n"/>
+      <c r="M10" s="6" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="11" s="56" spans="1:13" thickBot="1">
+      <c r="A11" s="11" t="n"/>
+      <c r="B11" s="47" t="s"/>
       <c r="C11" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="47"/>
+      <c r="D11" s="12" t="n"/>
+      <c r="E11" s="12" t="n"/>
+      <c r="F11" s="12" t="n"/>
+      <c r="G11" s="12" t="n"/>
+      <c r="H11" s="47" t="s"/>
       <c r="I11" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12"/>
-      <c r="L11" s="12"/>
-      <c r="M11" s="6"/>
-    </row>
-    <row r="12" spans="1:13" ht="15" customHeight="1" thickBot="1">
-      <c r="A12" s="11"/>
-      <c r="B12" s="47"/>
+      <c r="J11" s="12" t="n"/>
+      <c r="K11" s="12" t="n"/>
+      <c r="L11" s="12" t="n"/>
+      <c r="M11" s="6" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="12" s="56" spans="1:13" thickBot="1">
+      <c r="A12" s="11" t="n"/>
+      <c r="B12" s="47" t="s"/>
       <c r="C12" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="47"/>
+      <c r="D12" s="12" t="n"/>
+      <c r="E12" s="12" t="n"/>
+      <c r="F12" s="12" t="n"/>
+      <c r="G12" s="12" t="n"/>
+      <c r="H12" s="47" t="s"/>
       <c r="I12" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="J12" s="12"/>
-      <c r="K12" s="12"/>
-      <c r="L12" s="12"/>
-      <c r="M12" s="6"/>
-    </row>
-    <row r="13" spans="1:13" ht="15" customHeight="1" thickBot="1">
-      <c r="A13" s="11"/>
-      <c r="B13" s="47"/>
+      <c r="J12" s="12" t="n"/>
+      <c r="K12" s="12" t="n"/>
+      <c r="L12" s="12" t="n"/>
+      <c r="M12" s="6" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="13" s="56" spans="1:13" thickBot="1">
+      <c r="A13" s="11" t="n"/>
+      <c r="B13" s="47" t="s"/>
       <c r="C13" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="12"/>
-      <c r="H13" s="47"/>
+      <c r="D13" s="12" t="n"/>
+      <c r="E13" s="12" t="n"/>
+      <c r="F13" s="12" t="n"/>
+      <c r="G13" s="12" t="n"/>
+      <c r="H13" s="47" t="s"/>
       <c r="I13" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="J13" s="12"/>
-      <c r="K13" s="12"/>
-      <c r="L13" s="12"/>
-      <c r="M13" s="6"/>
-    </row>
-    <row r="14" spans="1:13" ht="15" customHeight="1" thickBot="1">
-      <c r="A14" s="11"/>
-      <c r="B14" s="47"/>
+      <c r="J13" s="12" t="n"/>
+      <c r="K13" s="12" t="n"/>
+      <c r="L13" s="12" t="n"/>
+      <c r="M13" s="6" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="14" s="56" spans="1:13" thickBot="1">
+      <c r="A14" s="11" t="n"/>
+      <c r="B14" s="47" t="s"/>
       <c r="C14" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="47"/>
+      <c r="D14" s="12" t="n"/>
+      <c r="E14" s="12" t="n"/>
+      <c r="F14" s="12" t="n"/>
+      <c r="G14" s="12" t="n"/>
+      <c r="H14" s="47" t="s"/>
       <c r="I14" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="J14" s="12"/>
-      <c r="K14" s="12"/>
-      <c r="L14" s="12"/>
-      <c r="M14" s="6"/>
-    </row>
-    <row r="15" spans="1:13" ht="15" customHeight="1" thickBot="1">
-      <c r="A15" s="11"/>
-      <c r="B15" s="47"/>
+      <c r="J14" s="12" t="n"/>
+      <c r="K14" s="12" t="n"/>
+      <c r="L14" s="12" t="n"/>
+      <c r="M14" s="6" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="15" s="56" spans="1:13" thickBot="1">
+      <c r="A15" s="11" t="n"/>
+      <c r="B15" s="47" t="s"/>
       <c r="C15" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="47"/>
+      <c r="D15" s="12" t="n"/>
+      <c r="E15" s="12" t="n"/>
+      <c r="F15" s="12" t="n"/>
+      <c r="G15" s="12" t="n"/>
+      <c r="H15" s="47" t="s"/>
       <c r="I15" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="J15" s="12"/>
-      <c r="K15" s="12"/>
-      <c r="L15" s="12"/>
-      <c r="M15" s="6"/>
-    </row>
-    <row r="16" spans="1:13" ht="15" customHeight="1" thickBot="1">
-      <c r="A16" s="11"/>
-      <c r="B16" s="47"/>
+      <c r="J15" s="12" t="n"/>
+      <c r="K15" s="12" t="n"/>
+      <c r="L15" s="12" t="n"/>
+      <c r="M15" s="6" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="16" s="56" spans="1:13" thickBot="1">
+      <c r="A16" s="11" t="n"/>
+      <c r="B16" s="47" t="s"/>
       <c r="C16" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="12"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="12"/>
-      <c r="H16" s="47"/>
+      <c r="D16" s="12" t="n"/>
+      <c r="E16" s="12" t="n"/>
+      <c r="F16" s="12" t="n"/>
+      <c r="G16" s="12" t="n"/>
+      <c r="H16" s="47" t="s"/>
       <c r="I16" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="J16" s="12"/>
-      <c r="K16" s="12"/>
-      <c r="L16" s="12"/>
-      <c r="M16" s="6"/>
-    </row>
-    <row r="17" spans="1:13" ht="15" customHeight="1" thickBot="1">
-      <c r="A17" s="11"/>
-      <c r="B17" s="47"/>
+      <c r="J16" s="12" t="n"/>
+      <c r="K16" s="12" t="n"/>
+      <c r="L16" s="12" t="n"/>
+      <c r="M16" s="6" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="17" s="56" spans="1:13" thickBot="1">
+      <c r="A17" s="11" t="n"/>
+      <c r="B17" s="47" t="s"/>
       <c r="C17" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="47"/>
+      <c r="D17" s="12" t="n"/>
+      <c r="E17" s="12" t="n"/>
+      <c r="F17" s="12" t="n"/>
+      <c r="G17" s="12" t="n"/>
+      <c r="H17" s="47" t="s"/>
       <c r="I17" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="J17" s="12"/>
-      <c r="K17" s="12"/>
-      <c r="L17" s="12"/>
-      <c r="M17" s="6"/>
-    </row>
-    <row r="18" spans="1:13" ht="15" customHeight="1" thickBot="1">
-      <c r="A18" s="11"/>
-      <c r="B18" s="47"/>
+      <c r="J17" s="12" t="n"/>
+      <c r="K17" s="12" t="n"/>
+      <c r="L17" s="12" t="n"/>
+      <c r="M17" s="6" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="18" s="56" spans="1:13" thickBot="1">
+      <c r="A18" s="11" t="n"/>
+      <c r="B18" s="47" t="s"/>
       <c r="C18" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
-      <c r="G18" s="12"/>
-      <c r="H18" s="47"/>
+      <c r="D18" s="12" t="n"/>
+      <c r="E18" s="12" t="n"/>
+      <c r="F18" s="12" t="n"/>
+      <c r="G18" s="12" t="n"/>
+      <c r="H18" s="47" t="s">
+        <v>22</v>
+      </c>
       <c r="I18" s="15" t="s">
-        <v>22</v>
-      </c>
-      <c r="J18" s="12"/>
-      <c r="K18" s="12"/>
-      <c r="L18" s="12"/>
-      <c r="M18" s="6"/>
-    </row>
-    <row r="19" spans="1:13" ht="15" customHeight="1" thickBot="1">
-      <c r="A19" s="11"/>
-      <c r="B19" s="47" t="s">
         <v>23</v>
       </c>
+      <c r="J18" s="12" t="n"/>
+      <c r="K18" s="12" t="n"/>
+      <c r="L18" s="12" t="n"/>
+      <c r="M18" s="6" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="19" s="56" spans="1:13" thickBot="1">
+      <c r="A19" s="11" t="n"/>
+      <c r="B19" s="47" t="s"/>
       <c r="C19" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="D19" s="16"/>
-      <c r="E19" s="16"/>
-      <c r="F19" s="16"/>
-      <c r="G19" s="16"/>
-      <c r="H19" s="49"/>
-      <c r="I19" s="16"/>
-      <c r="J19" s="16"/>
-      <c r="K19" s="16"/>
-      <c r="L19" s="12"/>
-      <c r="M19" s="6"/>
-    </row>
-    <row r="20" spans="1:13" ht="3.95" customHeight="1" thickBot="1">
-      <c r="A20" s="7"/>
-      <c r="B20" s="50"/>
-      <c r="C20" s="22"/>
-      <c r="D20" s="22"/>
-      <c r="E20" s="22"/>
-      <c r="F20" s="22"/>
-      <c r="G20" s="22"/>
-      <c r="H20" s="50"/>
-      <c r="I20" s="22"/>
-      <c r="J20" s="22"/>
-      <c r="K20" s="22"/>
-      <c r="L20" s="22"/>
-      <c r="M20" s="9"/>
-    </row>
-    <row r="21" spans="1:13" ht="3.95" customHeight="1">
-      <c r="A21" s="3"/>
-      <c r="B21" s="51"/>
-      <c r="C21" s="23"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="23"/>
-      <c r="G21" s="23"/>
-      <c r="H21" s="51"/>
-      <c r="I21" s="23"/>
-      <c r="J21" s="23"/>
-      <c r="K21" s="23"/>
-      <c r="L21" s="23"/>
-      <c r="M21" s="5"/>
-    </row>
-    <row r="22" spans="1:13" ht="15" customHeight="1">
-      <c r="A22" s="11"/>
-      <c r="B22" s="52"/>
-      <c r="C22" s="12"/>
+      <c r="D19" s="16" t="n"/>
+      <c r="E19" s="16" t="n"/>
+      <c r="F19" s="16" t="n"/>
+      <c r="G19" s="16" t="n"/>
+      <c r="H19" s="49" t="s"/>
+      <c r="I19" s="16" t="n"/>
+      <c r="J19" s="16" t="n"/>
+      <c r="K19" s="16" t="n"/>
+      <c r="L19" s="12" t="n"/>
+      <c r="M19" s="6" t="n"/>
+    </row>
+    <row customHeight="1" ht="3.95" r="20" s="56" spans="1:13" thickBot="1">
+      <c r="A20" s="7" t="n"/>
+      <c r="B20" s="50" t="s"/>
+      <c r="C20" s="22" t="n"/>
+      <c r="D20" s="22" t="n"/>
+      <c r="E20" s="22" t="n"/>
+      <c r="F20" s="22" t="n"/>
+      <c r="G20" s="22" t="n"/>
+      <c r="H20" s="50" t="s"/>
+      <c r="I20" s="22" t="n"/>
+      <c r="J20" s="22" t="n"/>
+      <c r="K20" s="22" t="n"/>
+      <c r="L20" s="22" t="n"/>
+      <c r="M20" s="9" t="n"/>
+    </row>
+    <row customHeight="1" ht="3.95" r="21" s="56" spans="1:13">
+      <c r="A21" s="3" t="n"/>
+      <c r="B21" s="51" t="s"/>
+      <c r="C21" s="23" t="n"/>
+      <c r="D21" s="23" t="n"/>
+      <c r="E21" s="23" t="n"/>
+      <c r="F21" s="23" t="n"/>
+      <c r="G21" s="23" t="n"/>
+      <c r="H21" s="51" t="s"/>
+      <c r="I21" s="23" t="n"/>
+      <c r="J21" s="23" t="n"/>
+      <c r="K21" s="23" t="n"/>
+      <c r="L21" s="23" t="n"/>
+      <c r="M21" s="5" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="22" s="56" spans="1:13">
+      <c r="A22" s="11" t="n"/>
+      <c r="B22" s="52" t="s"/>
+      <c r="C22" s="12" t="n"/>
       <c r="D22" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E22" s="16">
+      <c r="E22" s="16" t="n">
         <v>8000</v>
       </c>
-      <c r="F22" s="45">
+      <c r="F22" s="45" t="n">
         <v>1235</v>
       </c>
-      <c r="G22" s="12"/>
-      <c r="H22" s="52"/>
-      <c r="I22" s="12"/>
-      <c r="J22" s="12"/>
-      <c r="K22" s="12"/>
-      <c r="L22" s="12"/>
-      <c r="M22" s="6"/>
-    </row>
-    <row r="23" spans="1:13" ht="3.95" customHeight="1">
-      <c r="A23" s="18"/>
-      <c r="B23" s="53"/>
-      <c r="C23" s="24"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="24"/>
-      <c r="F23" s="24"/>
-      <c r="G23" s="24"/>
-      <c r="H23" s="53"/>
-      <c r="I23" s="24"/>
-      <c r="J23" s="24"/>
-      <c r="K23" s="24"/>
-      <c r="L23" s="24"/>
-      <c r="M23" s="19"/>
-    </row>
-    <row r="24" spans="1:13" ht="15" customHeight="1" thickBot="1">
-      <c r="A24" s="11"/>
-      <c r="B24" s="52"/>
+      <c r="G22" s="12" t="n"/>
+      <c r="H22" s="52" t="s"/>
+      <c r="I22" s="12" t="n"/>
+      <c r="J22" s="12" t="n"/>
+      <c r="K22" s="12" t="n"/>
+      <c r="L22" s="12" t="n"/>
+      <c r="M22" s="6" t="n"/>
+    </row>
+    <row customHeight="1" ht="3.95" r="23" s="56" spans="1:13">
+      <c r="A23" s="18" t="n"/>
+      <c r="B23" s="53" t="s"/>
+      <c r="C23" s="24" t="n"/>
+      <c r="D23" s="24" t="n"/>
+      <c r="E23" s="24" t="n"/>
+      <c r="F23" s="24" t="n"/>
+      <c r="G23" s="24" t="n"/>
+      <c r="H23" s="53" t="s"/>
+      <c r="I23" s="24" t="n"/>
+      <c r="J23" s="24" t="n"/>
+      <c r="K23" s="24" t="n"/>
+      <c r="L23" s="24" t="n"/>
+      <c r="M23" s="19" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="24" s="56" spans="1:13" thickBot="1">
+      <c r="A24" s="11" t="n"/>
+      <c r="B24" s="52" t="s"/>
       <c r="C24" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="52"/>
-      <c r="I24" s="12"/>
-      <c r="J24" s="12"/>
-      <c r="K24" s="12"/>
-      <c r="L24" s="12"/>
-      <c r="M24" s="6"/>
-    </row>
-    <row r="25" spans="1:13" ht="15" customHeight="1" thickBot="1">
-      <c r="A25" s="11"/>
-      <c r="B25" s="47"/>
+      <c r="D24" s="12" t="n"/>
+      <c r="E24" s="12" t="n"/>
+      <c r="F24" s="12" t="n"/>
+      <c r="G24" s="12" t="n"/>
+      <c r="H24" s="52" t="s"/>
+      <c r="I24" s="12" t="n"/>
+      <c r="J24" s="12" t="n"/>
+      <c r="K24" s="12" t="n"/>
+      <c r="L24" s="12" t="n"/>
+      <c r="M24" s="6" t="n"/>
+    </row>
+    <row customHeight="1" ht="15" r="25" s="56" spans="1:13" thickBot="1">
+      <c r="A25" s="11" t="n"/>
+      <c r="B25" s="47" t="s"/>
       <c r="C25" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
-      <c r="G25" s="12"/>
-      <c r="H25" s="47"/>
+      <c r="D25" s="12" t="n"/>
+      <c r="E25" s="12" t="n"/>
+      <c r="F25" s="12" t="n"/>
+      <c r="G25" s="12" t="n"/>
+      <c r="H25" s="47" t="s"/>
       <c r="I25" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="J25" s="12"/>
-      <c r="K25" s="12"/>
-      <c r="L25" s="12"/>
-      <c r="M25" s="6"/>
-    </row>
-    <row r="26" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A26" s="11"/>
-      <c r="B26" s="47"/>
+      <c r="J25" s="12" t="n"/>
+      <c r="K25" s="12" t="n"/>
+      <c r="L25" s="12" t="n"/>
+      <c r="M25" s="6" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="26" s="56" spans="1:13" thickBot="1">
+      <c r="A26" s="11" t="n"/>
+      <c r="B26" s="47" t="s"/>
       <c r="C26" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="D26" s="12"/>
-      <c r="E26" s="12"/>
-      <c r="F26" s="12"/>
-      <c r="G26" s="12"/>
-      <c r="H26" s="47"/>
+      <c r="D26" s="12" t="n"/>
+      <c r="E26" s="12" t="n"/>
+      <c r="F26" s="12" t="n"/>
+      <c r="G26" s="12" t="n"/>
+      <c r="H26" s="47" t="s"/>
       <c r="I26" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="J26" s="12"/>
-      <c r="K26" s="12"/>
-      <c r="L26" s="12"/>
-      <c r="M26" s="6"/>
-    </row>
-    <row r="27" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A27" s="11"/>
-      <c r="B27" s="47"/>
+      <c r="J26" s="12" t="n"/>
+      <c r="K26" s="12" t="n"/>
+      <c r="L26" s="12" t="n"/>
+      <c r="M26" s="6" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="27" s="56" spans="1:13" thickBot="1">
+      <c r="A27" s="11" t="n"/>
+      <c r="B27" s="47" t="s"/>
       <c r="C27" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="12"/>
-      <c r="G27" s="12"/>
-      <c r="H27" s="47"/>
+      <c r="D27" s="12" t="n"/>
+      <c r="E27" s="12" t="n"/>
+      <c r="F27" s="12" t="n"/>
+      <c r="G27" s="12" t="n"/>
+      <c r="H27" s="47" t="s"/>
       <c r="I27" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="J27" s="12"/>
-      <c r="K27" s="12"/>
-      <c r="L27" s="12"/>
-      <c r="M27" s="6"/>
-    </row>
-    <row r="28" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A28" s="11"/>
-      <c r="B28" s="47"/>
+      <c r="J27" s="12" t="n"/>
+      <c r="K27" s="12" t="n"/>
+      <c r="L27" s="12" t="n"/>
+      <c r="M27" s="6" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="28" s="56" spans="1:13" thickBot="1">
+      <c r="A28" s="11" t="n"/>
+      <c r="B28" s="47" t="s"/>
       <c r="C28" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="D28" s="12"/>
-      <c r="E28" s="12"/>
-      <c r="F28" s="12"/>
-      <c r="G28" s="12"/>
-      <c r="H28" s="47"/>
+      <c r="D28" s="12" t="n"/>
+      <c r="E28" s="12" t="n"/>
+      <c r="F28" s="12" t="n"/>
+      <c r="G28" s="12" t="n"/>
+      <c r="H28" s="47" t="s"/>
       <c r="I28" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="J28" s="12"/>
-      <c r="K28" s="12"/>
-      <c r="L28" s="12"/>
-      <c r="M28" s="6"/>
-    </row>
-    <row r="29" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A29" s="11"/>
-      <c r="B29" s="47"/>
+      <c r="J28" s="12" t="n"/>
+      <c r="K28" s="12" t="n"/>
+      <c r="L28" s="12" t="n"/>
+      <c r="M28" s="6" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="29" s="56" spans="1:13" thickBot="1">
+      <c r="A29" s="11" t="n"/>
+      <c r="B29" s="47" t="s"/>
       <c r="C29" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="D29" s="16"/>
-      <c r="E29" s="16"/>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
-      <c r="H29" s="49"/>
-      <c r="I29" s="16"/>
-      <c r="J29" s="16"/>
-      <c r="K29" s="16"/>
-      <c r="L29" s="12"/>
-      <c r="M29" s="6"/>
-    </row>
-    <row r="30" spans="1:13" ht="3.95" customHeight="1">
-      <c r="A30" s="20"/>
-      <c r="B30" s="49"/>
-      <c r="C30" s="16"/>
-      <c r="D30" s="16"/>
-      <c r="E30" s="16"/>
-      <c r="F30" s="16"/>
-      <c r="G30" s="16"/>
-      <c r="H30" s="49"/>
-      <c r="I30" s="16"/>
-      <c r="J30" s="16"/>
-      <c r="K30" s="16"/>
-      <c r="L30" s="16"/>
-      <c r="M30" s="21"/>
-    </row>
-    <row r="31" spans="1:13" ht="3.95" customHeight="1">
-      <c r="A31" s="11"/>
-      <c r="B31" s="52"/>
-      <c r="C31" s="12"/>
-      <c r="D31" s="12"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="12"/>
-      <c r="G31" s="12"/>
-      <c r="H31" s="52"/>
-      <c r="I31" s="12"/>
-      <c r="J31" s="12"/>
-      <c r="K31" s="12"/>
-      <c r="L31" s="12"/>
-      <c r="M31" s="6"/>
-    </row>
-    <row r="32" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A32" s="11"/>
-      <c r="B32" s="52"/>
+      <c r="D29" s="16" t="n"/>
+      <c r="E29" s="16" t="n"/>
+      <c r="F29" s="16" t="n"/>
+      <c r="G29" s="16" t="n"/>
+      <c r="H29" s="49" t="s"/>
+      <c r="I29" s="16" t="n"/>
+      <c r="J29" s="16" t="n"/>
+      <c r="K29" s="16" t="n"/>
+      <c r="L29" s="12" t="n"/>
+      <c r="M29" s="6" t="n"/>
+    </row>
+    <row customHeight="1" ht="3.95" r="30" s="56" spans="1:13">
+      <c r="A30" s="20" t="n"/>
+      <c r="B30" s="49" t="s"/>
+      <c r="C30" s="16" t="n"/>
+      <c r="D30" s="16" t="n"/>
+      <c r="E30" s="16" t="n"/>
+      <c r="F30" s="16" t="n"/>
+      <c r="G30" s="16" t="n"/>
+      <c r="H30" s="49" t="s"/>
+      <c r="I30" s="16" t="n"/>
+      <c r="J30" s="16" t="n"/>
+      <c r="K30" s="16" t="n"/>
+      <c r="L30" s="16" t="n"/>
+      <c r="M30" s="21" t="n"/>
+    </row>
+    <row customHeight="1" ht="3.95" r="31" s="56" spans="1:13">
+      <c r="A31" s="11" t="n"/>
+      <c r="B31" s="52" t="s"/>
+      <c r="C31" s="12" t="n"/>
+      <c r="D31" s="12" t="n"/>
+      <c r="E31" s="12" t="n"/>
+      <c r="F31" s="12" t="n"/>
+      <c r="G31" s="12" t="n"/>
+      <c r="H31" s="52" t="s"/>
+      <c r="I31" s="12" t="n"/>
+      <c r="J31" s="12" t="n"/>
+      <c r="K31" s="12" t="n"/>
+      <c r="L31" s="12" t="n"/>
+      <c r="M31" s="6" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="32" s="56" spans="1:13" thickBot="1">
+      <c r="A32" s="11" t="n"/>
+      <c r="B32" s="52" t="s"/>
       <c r="C32" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D32" s="12"/>
-      <c r="E32" s="12"/>
-      <c r="F32" s="12"/>
-      <c r="G32" s="12"/>
-      <c r="H32" s="52"/>
-      <c r="I32" s="12"/>
-      <c r="J32" s="12"/>
-      <c r="K32" s="12"/>
-      <c r="L32" s="12"/>
-      <c r="M32" s="6"/>
-    </row>
-    <row r="33" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A33" s="11"/>
-      <c r="B33" s="47"/>
+      <c r="D32" s="12" t="n"/>
+      <c r="E32" s="12" t="n"/>
+      <c r="F32" s="12" t="n"/>
+      <c r="G32" s="12" t="n"/>
+      <c r="H32" s="52" t="s"/>
+      <c r="I32" s="12" t="n"/>
+      <c r="J32" s="12" t="n"/>
+      <c r="K32" s="12" t="n"/>
+      <c r="L32" s="12" t="n"/>
+      <c r="M32" s="6" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="33" s="56" spans="1:13" thickBot="1">
+      <c r="A33" s="11" t="n"/>
+      <c r="B33" s="47" t="s"/>
       <c r="C33" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="D33" s="12"/>
-      <c r="E33" s="12"/>
-      <c r="F33" s="12"/>
-      <c r="G33" s="12"/>
+      <c r="D33" s="12" t="n"/>
+      <c r="E33" s="12" t="n"/>
+      <c r="F33" s="12" t="n"/>
+      <c r="G33" s="12" t="n"/>
       <c r="H33" s="47" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I33" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="J33" s="12"/>
-      <c r="K33" s="12"/>
-      <c r="L33" s="12"/>
-      <c r="M33" s="6"/>
-    </row>
-    <row r="34" spans="1:13" ht="15.75" customHeight="1" thickBot="1">
-      <c r="A34" s="11"/>
-      <c r="B34" s="47"/>
+      <c r="J33" s="12" t="n"/>
+      <c r="K33" s="12" t="n"/>
+      <c r="L33" s="12" t="n"/>
+      <c r="M33" s="6" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="34" s="56" spans="1:13" thickBot="1">
+      <c r="A34" s="11" t="n"/>
+      <c r="B34" s="47" t="s"/>
       <c r="C34" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="D34" s="16"/>
-      <c r="E34" s="16"/>
-      <c r="F34" s="16"/>
-      <c r="G34" s="16"/>
-      <c r="H34" s="16"/>
-      <c r="I34" s="16"/>
-      <c r="J34" s="16"/>
-      <c r="K34" s="16"/>
-      <c r="L34" s="12"/>
-      <c r="M34" s="6"/>
-    </row>
-    <row r="35" spans="1:13" ht="3.95" customHeight="1" thickBot="1">
-      <c r="A35" s="7"/>
-      <c r="B35" s="22"/>
-      <c r="C35" s="22"/>
-      <c r="D35" s="22"/>
-      <c r="E35" s="22"/>
-      <c r="F35" s="22"/>
-      <c r="G35" s="22"/>
-      <c r="H35" s="22"/>
-      <c r="I35" s="22"/>
-      <c r="J35" s="22"/>
-      <c r="K35" s="22"/>
-      <c r="L35" s="22"/>
-      <c r="M35" s="9"/>
-    </row>
-    <row r="36" spans="1:13" ht="3.95" customHeight="1">
-      <c r="B36" s="12"/>
-      <c r="C36" s="12"/>
-      <c r="D36" s="12"/>
-      <c r="E36" s="12"/>
-      <c r="F36" s="12"/>
-      <c r="G36" s="12"/>
-      <c r="H36" s="12"/>
-      <c r="I36" s="12"/>
-      <c r="J36" s="12"/>
-      <c r="K36" s="12"/>
-      <c r="L36" s="12"/>
+      <c r="D34" s="16" t="n"/>
+      <c r="E34" s="16" t="n"/>
+      <c r="F34" s="16" t="n"/>
+      <c r="G34" s="16" t="n"/>
+      <c r="H34" s="16" t="s"/>
+      <c r="I34" s="16" t="n"/>
+      <c r="J34" s="16" t="n"/>
+      <c r="K34" s="16" t="n"/>
+      <c r="L34" s="12" t="n"/>
+      <c r="M34" s="6" t="n"/>
+    </row>
+    <row customHeight="1" ht="3.95" r="35" s="56" spans="1:13" thickBot="1">
+      <c r="A35" s="7" t="n"/>
+      <c r="B35" s="22" t="n"/>
+      <c r="C35" s="22" t="n"/>
+      <c r="D35" s="22" t="n"/>
+      <c r="E35" s="22" t="n"/>
+      <c r="F35" s="22" t="n"/>
+      <c r="G35" s="22" t="n"/>
+      <c r="H35" s="22" t="n"/>
+      <c r="I35" s="22" t="n"/>
+      <c r="J35" s="22" t="n"/>
+      <c r="K35" s="22" t="n"/>
+      <c r="L35" s="22" t="n"/>
+      <c r="M35" s="9" t="n"/>
+    </row>
+    <row customHeight="1" ht="3.95" r="36" s="56" spans="1:13">
+      <c r="B36" s="12" t="n"/>
+      <c r="C36" s="12" t="n"/>
+      <c r="D36" s="12" t="n"/>
+      <c r="E36" s="12" t="n"/>
+      <c r="F36" s="12" t="n"/>
+      <c r="G36" s="12" t="n"/>
+      <c r="H36" s="12" t="n"/>
+      <c r="I36" s="12" t="n"/>
+      <c r="J36" s="12" t="n"/>
+      <c r="K36" s="12" t="n"/>
+      <c r="L36" s="12" t="n"/>
     </row>
     <row r="37" spans="1:13">
       <c r="C37" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D37" s="12"/>
-      <c r="E37" s="12"/>
-      <c r="F37" s="12"/>
-      <c r="G37" s="12"/>
-      <c r="H37" s="12"/>
-      <c r="I37" s="12"/>
-      <c r="J37" s="12"/>
-      <c r="K37" s="12"/>
-      <c r="L37" s="12"/>
+      <c r="D37" s="12" t="n"/>
+      <c r="E37" s="12" t="n"/>
+      <c r="F37" s="12" t="n"/>
+      <c r="G37" s="12" t="n"/>
+      <c r="H37" s="12" t="n"/>
+      <c r="I37" s="12" t="n"/>
+      <c r="J37" s="12" t="n"/>
+      <c r="K37" s="12" t="n"/>
+      <c r="L37" s="12" t="n"/>
     </row>
     <row r="38" spans="1:13">
-      <c r="B38" s="25"/>
+      <c r="B38" s="25" t="n"/>
       <c r="C38" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="D38" s="27"/>
-      <c r="E38" s="28"/>
-      <c r="F38" s="29"/>
+      <c r="D38" s="27" t="n"/>
+      <c r="E38" s="28" t="n"/>
+      <c r="F38" s="29" t="n"/>
       <c r="G38" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="H38" s="31"/>
-      <c r="I38" s="28"/>
+      <c r="H38" s="31" t="n"/>
+      <c r="I38" s="28" t="n"/>
       <c r="J38" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="K38" s="31"/>
+      <c r="K38" s="31" t="n"/>
       <c r="L38" s="43" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="39" spans="1:13">
-      <c r="B39" s="28"/>
-      <c r="C39" s="29"/>
-      <c r="D39" s="31"/>
-      <c r="E39" s="25"/>
-      <c r="F39" s="32"/>
-      <c r="G39" s="32"/>
-      <c r="H39" s="27"/>
-      <c r="I39" s="25"/>
-      <c r="J39" s="32"/>
-      <c r="K39" s="27"/>
-      <c r="L39" s="34"/>
+      <c r="B39" s="28" t="n"/>
+      <c r="C39" s="29" t="n"/>
+      <c r="D39" s="31" t="n"/>
+      <c r="E39" s="25" t="n"/>
+      <c r="F39" s="32" t="n"/>
+      <c r="G39" s="32" t="n"/>
+      <c r="H39" s="27" t="n"/>
+      <c r="I39" s="25" t="n"/>
+      <c r="J39" s="32" t="n"/>
+      <c r="K39" s="27" t="n"/>
+      <c r="L39" s="34" t="n"/>
     </row>
     <row r="40" spans="1:13">
-      <c r="B40" s="25"/>
-      <c r="C40" s="32"/>
-      <c r="D40" s="27"/>
-      <c r="E40" s="25"/>
-      <c r="F40" s="32"/>
-      <c r="G40" s="32"/>
-      <c r="H40" s="27"/>
-      <c r="I40" s="25"/>
-      <c r="J40" s="32"/>
-      <c r="K40" s="27"/>
-      <c r="L40" s="34"/>
+      <c r="B40" s="25" t="n"/>
+      <c r="C40" s="32" t="n"/>
+      <c r="D40" s="27" t="n"/>
+      <c r="E40" s="25" t="n"/>
+      <c r="F40" s="32" t="n"/>
+      <c r="G40" s="32" t="n"/>
+      <c r="H40" s="27" t="n"/>
+      <c r="I40" s="25" t="n"/>
+      <c r="J40" s="32" t="n"/>
+      <c r="K40" s="27" t="n"/>
+      <c r="L40" s="34" t="n"/>
     </row>
     <row r="41" spans="1:13">
-      <c r="B41" s="25"/>
-      <c r="C41" s="32"/>
-      <c r="D41" s="27"/>
-      <c r="E41" s="25"/>
-      <c r="F41" s="32"/>
-      <c r="G41" s="32"/>
-      <c r="H41" s="27"/>
-      <c r="I41" s="25"/>
-      <c r="J41" s="32"/>
-      <c r="K41" s="27"/>
-      <c r="L41" s="34"/>
+      <c r="B41" s="25" t="n"/>
+      <c r="C41" s="32" t="n"/>
+      <c r="D41" s="27" t="n"/>
+      <c r="E41" s="25" t="n"/>
+      <c r="F41" s="32" t="n"/>
+      <c r="G41" s="32" t="n"/>
+      <c r="H41" s="27" t="n"/>
+      <c r="I41" s="25" t="n"/>
+      <c r="J41" s="32" t="n"/>
+      <c r="K41" s="27" t="n"/>
+      <c r="L41" s="34" t="n"/>
     </row>
     <row r="42" spans="1:13">
-      <c r="B42" s="25"/>
-      <c r="C42" s="32"/>
-      <c r="D42" s="27"/>
-      <c r="E42" s="25"/>
-      <c r="F42" s="32"/>
-      <c r="G42" s="32"/>
-      <c r="H42" s="27"/>
-      <c r="I42" s="25"/>
-      <c r="J42" s="32"/>
-      <c r="K42" s="27"/>
-      <c r="L42" s="34"/>
+      <c r="B42" s="25" t="n"/>
+      <c r="C42" s="32" t="n"/>
+      <c r="D42" s="27" t="n"/>
+      <c r="E42" s="25" t="n"/>
+      <c r="F42" s="32" t="n"/>
+      <c r="G42" s="32" t="n"/>
+      <c r="H42" s="27" t="n"/>
+      <c r="I42" s="25" t="n"/>
+      <c r="J42" s="32" t="n"/>
+      <c r="K42" s="27" t="n"/>
+      <c r="L42" s="34" t="n"/>
     </row>
     <row r="43" spans="1:13">
-      <c r="B43" s="25"/>
-      <c r="C43" s="32"/>
-      <c r="D43" s="27"/>
-      <c r="E43" s="25"/>
-      <c r="F43" s="32"/>
-      <c r="G43" s="32"/>
-      <c r="H43" s="27"/>
-      <c r="I43" s="25"/>
-      <c r="J43" s="32"/>
-      <c r="K43" s="27"/>
-      <c r="L43" s="34"/>
+      <c r="B43" s="25" t="n"/>
+      <c r="C43" s="32" t="n"/>
+      <c r="D43" s="27" t="n"/>
+      <c r="E43" s="25" t="n"/>
+      <c r="F43" s="32" t="n"/>
+      <c r="G43" s="32" t="n"/>
+      <c r="H43" s="27" t="n"/>
+      <c r="I43" s="25" t="n"/>
+      <c r="J43" s="32" t="n"/>
+      <c r="K43" s="27" t="n"/>
+      <c r="L43" s="34" t="n"/>
     </row>
     <row r="44" spans="1:13">
-      <c r="B44" s="25"/>
-      <c r="C44" s="32"/>
-      <c r="D44" s="27"/>
-      <c r="E44" s="25"/>
-      <c r="F44" s="32"/>
-      <c r="G44" s="32"/>
-      <c r="H44" s="27"/>
-      <c r="I44" s="25"/>
-      <c r="J44" s="32"/>
-      <c r="K44" s="27"/>
-      <c r="L44" s="34"/>
-    </row>
-    <row r="45" spans="1:13" ht="15.75" customHeight="1" thickBot="1"/>
-    <row r="46" spans="1:13" ht="3.95" customHeight="1">
-      <c r="A46" s="3"/>
-      <c r="B46" s="4"/>
-      <c r="C46" s="4"/>
-      <c r="D46" s="4"/>
-      <c r="E46" s="4"/>
-      <c r="F46" s="4"/>
-      <c r="G46" s="4"/>
-      <c r="H46" s="4"/>
-      <c r="I46" s="4"/>
-      <c r="J46" s="4"/>
-      <c r="K46" s="4"/>
-      <c r="L46" s="4"/>
-      <c r="M46" s="5"/>
+      <c r="B44" s="25" t="n"/>
+      <c r="C44" s="32" t="n"/>
+      <c r="D44" s="27" t="n"/>
+      <c r="E44" s="25" t="n"/>
+      <c r="F44" s="32" t="n"/>
+      <c r="G44" s="32" t="n"/>
+      <c r="H44" s="27" t="n"/>
+      <c r="I44" s="25" t="n"/>
+      <c r="J44" s="32" t="n"/>
+      <c r="K44" s="27" t="n"/>
+      <c r="L44" s="34" t="n"/>
+    </row>
+    <row customHeight="1" ht="15.75" r="45" s="56" spans="1:13" thickBot="1"/>
+    <row customHeight="1" ht="3.95" r="46" s="56" spans="1:13">
+      <c r="A46" s="3" t="n"/>
+      <c r="B46" s="4" t="n"/>
+      <c r="C46" s="4" t="n"/>
+      <c r="D46" s="4" t="n"/>
+      <c r="E46" s="4" t="n"/>
+      <c r="F46" s="4" t="n"/>
+      <c r="G46" s="4" t="n"/>
+      <c r="H46" s="4" t="n"/>
+      <c r="I46" s="4" t="n"/>
+      <c r="J46" s="4" t="n"/>
+      <c r="K46" s="4" t="n"/>
+      <c r="L46" s="4" t="n"/>
+      <c r="M46" s="5" t="n"/>
     </row>
     <row r="47" spans="1:13">
-      <c r="A47" s="11"/>
+      <c r="A47" s="11" t="n"/>
       <c r="D47" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="E47" s="2"/>
-      <c r="F47" s="2"/>
+      <c r="E47" s="2" t="n"/>
+      <c r="F47" s="2" t="n"/>
       <c r="J47" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="K47" s="16"/>
-      <c r="M47" s="6"/>
-    </row>
-    <row r="48" spans="1:13" ht="3.95" customHeight="1" thickBot="1">
-      <c r="A48" s="7"/>
-      <c r="B48" s="8"/>
-      <c r="C48" s="8"/>
-      <c r="D48" s="8"/>
-      <c r="E48" s="8"/>
-      <c r="F48" s="8"/>
-      <c r="G48" s="8"/>
-      <c r="H48" s="8"/>
-      <c r="I48" s="8"/>
-      <c r="J48" s="8"/>
-      <c r="K48" s="8"/>
-      <c r="L48" s="8"/>
-      <c r="M48" s="9"/>
-    </row>
-    <row r="50" spans="1:13" ht="3.95" customHeight="1">
-      <c r="A50" s="36"/>
-      <c r="B50" s="37"/>
-      <c r="C50" s="37"/>
-      <c r="D50" s="37"/>
-      <c r="E50" s="37"/>
-      <c r="F50" s="37"/>
-      <c r="G50" s="37"/>
-      <c r="H50" s="37"/>
-      <c r="I50" s="37"/>
-      <c r="J50" s="37"/>
-      <c r="K50" s="37"/>
-      <c r="L50" s="37"/>
-      <c r="M50" s="38"/>
+      <c r="K47" s="16" t="n"/>
+      <c r="M47" s="6" t="n"/>
+    </row>
+    <row customHeight="1" ht="3.95" r="48" s="56" spans="1:13" thickBot="1">
+      <c r="A48" s="7" t="n"/>
+      <c r="B48" s="8" t="n"/>
+      <c r="C48" s="8" t="n"/>
+      <c r="D48" s="8" t="n"/>
+      <c r="E48" s="8" t="n"/>
+      <c r="F48" s="8" t="n"/>
+      <c r="G48" s="8" t="n"/>
+      <c r="H48" s="8" t="n"/>
+      <c r="I48" s="8" t="n"/>
+      <c r="J48" s="8" t="n"/>
+      <c r="K48" s="8" t="n"/>
+      <c r="L48" s="8" t="n"/>
+      <c r="M48" s="9" t="n"/>
+    </row>
+    <row customHeight="1" ht="3.95" r="50" s="56" spans="1:13">
+      <c r="A50" s="36" t="n"/>
+      <c r="B50" s="37" t="n"/>
+      <c r="C50" s="37" t="n"/>
+      <c r="D50" s="37" t="n"/>
+      <c r="E50" s="37" t="n"/>
+      <c r="F50" s="37" t="n"/>
+      <c r="G50" s="37" t="n"/>
+      <c r="H50" s="37" t="n"/>
+      <c r="I50" s="37" t="n"/>
+      <c r="J50" s="37" t="n"/>
+      <c r="K50" s="37" t="n"/>
+      <c r="L50" s="37" t="n"/>
+      <c r="M50" s="38" t="n"/>
     </row>
     <row r="51" spans="1:13">
-      <c r="A51" s="39"/>
+      <c r="A51" s="39" t="n"/>
       <c r="C51" s="48" t="s">
         <v>44</v>
       </c>
-      <c r="M51" s="40"/>
+      <c r="M51" s="40" t="n"/>
     </row>
     <row r="52" spans="1:13">
-      <c r="A52" s="39"/>
+      <c r="A52" s="39" t="n"/>
       <c r="C52" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="D52" s="55">
-        <v>896321475</v>
-      </c>
-      <c r="E52" s="56"/>
-      <c r="M52" s="40"/>
+      <c r="D52" s="55" t="n">
+        <v>123456789</v>
+      </c>
+      <c r="M52" s="40" t="n"/>
     </row>
     <row r="53" spans="1:13">
-      <c r="A53" s="39"/>
-      <c r="M53" s="40"/>
+      <c r="A53" s="39" t="n"/>
+      <c r="M53" s="40" t="n"/>
     </row>
     <row r="54" spans="1:13">
-      <c r="A54" s="39"/>
-      <c r="M54" s="40"/>
+      <c r="A54" s="39" t="n"/>
+      <c r="M54" s="40" t="n"/>
     </row>
     <row r="55" spans="1:13">
-      <c r="A55" s="41"/>
-      <c r="B55" s="17"/>
-      <c r="C55" s="17"/>
-      <c r="D55" s="17"/>
-      <c r="E55" s="17"/>
-      <c r="F55" s="17"/>
-      <c r="G55" s="17"/>
-      <c r="H55" s="17"/>
-      <c r="I55" s="17"/>
-      <c r="J55" s="17"/>
-      <c r="K55" s="17"/>
-      <c r="L55" s="17"/>
-      <c r="M55" s="42"/>
+      <c r="A55" s="41" t="n"/>
+      <c r="B55" s="17" t="n"/>
+      <c r="C55" s="17" t="n"/>
+      <c r="D55" s="17" t="n"/>
+      <c r="E55" s="17" t="n"/>
+      <c r="F55" s="17" t="n"/>
+      <c r="G55" s="17" t="n"/>
+      <c r="H55" s="17" t="n"/>
+      <c r="I55" s="17" t="n"/>
+      <c r="J55" s="17" t="n"/>
+      <c r="K55" s="17" t="n"/>
+      <c r="L55" s="17" t="n"/>
+      <c r="M55" s="42" t="n"/>
     </row>
     <row r="56" spans="1:13">
       <c r="C56" t="s">
@@ -1761,7 +1764,7 @@
   <mergeCells count="1">
     <mergeCell ref="D52:E52"/>
   </mergeCells>
-  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="96" orientation="portrait" verticalDpi="300"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.25" right="0.25" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" scale="96" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
change position for notes
</commit_message>
<xml_diff>
--- a/f2-02-04-5.xlsx
+++ b/f2-02-04-5.xlsx
@@ -9,7 +9,7 @@
     <sheet name="1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -22,13 +22,13 @@
     <t>дата:</t>
   </si>
   <si>
-    <t>15/01/2018</t>
+    <t>16/01/2018</t>
   </si>
   <si>
     <t>час:</t>
   </si>
   <si>
-    <t>14:40</t>
+    <t>10:06</t>
   </si>
   <si>
     <t>Автор повідомлення:</t>
@@ -82,10 +82,10 @@
     <t>Рекваліфікація / EMPB</t>
   </si>
   <si>
+    <t>Обладнання не вмикається / не продукує виріб</t>
+  </si>
+  <si>
     <t>X</t>
-  </si>
-  <si>
-    <t>Обладнання не вмикається / не продукує виріб</t>
   </si>
   <si>
     <t>Інше:</t>
@@ -227,7 +227,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -248,21 +248,6 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top style="medium">
         <color indexed="64"/>
@@ -550,23 +535,23 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="59">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="2" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="3" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="4" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="5" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="6" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="7" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="8" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="9" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="10" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="5" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -582,61 +567,61 @@
     <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf borderId="10" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="11" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="12" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="13" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="14" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="15" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="9" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="8" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="4" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="3" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="11" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="10" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="16" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="17" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="18" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="19" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="20" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="20" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="21" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf applyAlignment="1" borderId="17" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="18" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="19" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf applyAlignment="1" borderId="20" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="21" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="21" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="22" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="18" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf applyAlignment="1" borderId="21" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="16" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="15" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
+    <xf borderId="22" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="23" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="24" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="25" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="26" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="27" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf borderId="28" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf borderId="29" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="16" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="15" fillId="0" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
@@ -648,25 +633,22 @@
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="3" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf applyAlignment="1" borderId="2" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
     <xf applyAlignment="1" borderId="1" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="9" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="8" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="4" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="3" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf applyAlignment="1" borderId="11" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf applyAlignment="1" borderId="10" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
@@ -674,9 +656,18 @@
       <alignment horizontal="left"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="15" fillId="0" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Обычный" xfId="0"/>
+    <cellStyle builtinId="0" name="Звичайний" xfId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
@@ -973,29 +964,29 @@
   </sheetPr>
   <dimension ref="A3:M56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" zoomScaleSheetLayoutView="115">
-      <selection activeCell="F40" sqref="F40"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0" zoomScaleSheetLayoutView="115">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col customWidth="1" max="1" min="1" style="56" width="1.140625"/>
-    <col customWidth="1" max="2" min="2" style="56" width="4.140625"/>
-    <col customWidth="1" max="7" min="7" style="56" width="3.5703125"/>
-    <col customWidth="1" max="8" min="8" style="56" width="4.140625"/>
-    <col customWidth="1" max="11" min="11" style="56" width="14.85546875"/>
-    <col customWidth="1" max="12" min="12" style="56" width="8.140625"/>
-    <col customWidth="1" max="13" min="13" style="56" width="1.85546875"/>
-    <col customWidth="1" max="14" min="14" style="56" width="2.28515625"/>
+    <col customWidth="1" max="1" min="1" style="55" width="1.140625"/>
+    <col customWidth="1" max="2" min="2" style="55" width="4.140625"/>
+    <col customWidth="1" max="7" min="7" style="55" width="3.5703125"/>
+    <col customWidth="1" max="8" min="8" style="55" width="4.140625"/>
+    <col customWidth="1" max="11" min="11" style="55" width="14.85546875"/>
+    <col customWidth="1" max="12" min="12" style="55" width="8.140625"/>
+    <col customWidth="1" max="13" min="13" style="55" width="1.85546875"/>
+    <col customWidth="1" max="14" min="14" style="55" width="2.28515625"/>
   </cols>
   <sheetData>
-    <row customHeight="1" ht="20.25" r="3" s="56" spans="1:13">
+    <row customHeight="1" ht="20.25" r="3" s="55" spans="1:13">
       <c r="F3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row customHeight="1" ht="15.75" r="5" s="56" spans="1:13" thickBot="1"/>
-    <row customHeight="1" ht="3.95" r="6" s="56" spans="1:13">
+    <row customHeight="1" ht="15.75" r="5" s="55" spans="1:13" thickBot="1"/>
+    <row customHeight="1" ht="3.95" r="6" s="55" spans="1:13">
       <c r="A6" s="3" t="n"/>
       <c r="B6" s="4" t="n"/>
       <c r="C6" s="4" t="n"/>
@@ -1010,7 +1001,7 @@
       <c r="L6" s="4" t="n"/>
       <c r="M6" s="5" t="n"/>
     </row>
-    <row r="7" spans="1:13">
+    <row customHeight="1" ht="20.1" r="7" s="55" spans="1:13">
       <c r="A7" s="11" t="s">
         <v>1</v>
       </c>
@@ -1032,12 +1023,12 @@
         <v>5</v>
       </c>
       <c r="K7" s="44" t="n">
-        <v>3012</v>
+        <v>3333</v>
       </c>
       <c r="L7" s="12" t="n"/>
       <c r="M7" s="6" t="n"/>
     </row>
-    <row customHeight="1" ht="3.95" r="8" s="56" spans="1:13" thickBot="1">
+    <row customHeight="1" ht="3.95" r="8" s="55" spans="1:13" thickBot="1">
       <c r="A8" s="7" t="n"/>
       <c r="B8" s="22" t="n"/>
       <c r="C8" s="22" t="n"/>
@@ -1052,7 +1043,7 @@
       <c r="L8" s="22" t="n"/>
       <c r="M8" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="3.95" r="9" s="56" spans="1:13">
+    <row customHeight="1" ht="3.95" r="9" s="55" spans="1:13">
       <c r="A9" s="3" t="n"/>
       <c r="B9" s="23" t="n"/>
       <c r="C9" s="23" t="n"/>
@@ -1067,9 +1058,9 @@
       <c r="L9" s="23" t="n"/>
       <c r="M9" s="5" t="n"/>
     </row>
-    <row customHeight="1" ht="15.75" r="10" s="56" spans="1:13" thickBot="1">
+    <row customHeight="1" ht="20.1" r="10" s="55" spans="1:13">
       <c r="A10" s="11" t="n"/>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="56" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="12" t="n"/>
@@ -1083,9 +1074,9 @@
       <c r="L10" s="12" t="n"/>
       <c r="M10" s="6" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="11" s="56" spans="1:13" thickBot="1">
+    <row customHeight="1" ht="20.1" r="11" s="55" spans="1:13">
       <c r="A11" s="11" t="n"/>
-      <c r="B11" s="47" t="s"/>
+      <c r="B11" s="58" t="s"/>
       <c r="C11" s="14" t="s">
         <v>7</v>
       </c>
@@ -1093,7 +1084,7 @@
       <c r="E11" s="12" t="n"/>
       <c r="F11" s="12" t="n"/>
       <c r="G11" s="12" t="n"/>
-      <c r="H11" s="47" t="s"/>
+      <c r="H11" s="58" t="s"/>
       <c r="I11" s="14" t="s">
         <v>8</v>
       </c>
@@ -1102,9 +1093,9 @@
       <c r="L11" s="12" t="n"/>
       <c r="M11" s="6" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="12" s="56" spans="1:13" thickBot="1">
+    <row customHeight="1" ht="20.1" r="12" s="55" spans="1:13">
       <c r="A12" s="11" t="n"/>
-      <c r="B12" s="47" t="s"/>
+      <c r="B12" s="58" t="s"/>
       <c r="C12" s="14" t="s">
         <v>9</v>
       </c>
@@ -1112,7 +1103,7 @@
       <c r="E12" s="12" t="n"/>
       <c r="F12" s="12" t="n"/>
       <c r="G12" s="12" t="n"/>
-      <c r="H12" s="47" t="s"/>
+      <c r="H12" s="58" t="s"/>
       <c r="I12" s="14" t="s">
         <v>10</v>
       </c>
@@ -1121,9 +1112,9 @@
       <c r="L12" s="12" t="n"/>
       <c r="M12" s="6" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="13" s="56" spans="1:13" thickBot="1">
+    <row customHeight="1" ht="20.1" r="13" s="55" spans="1:13">
       <c r="A13" s="11" t="n"/>
-      <c r="B13" s="47" t="s"/>
+      <c r="B13" s="58" t="s"/>
       <c r="C13" s="14" t="s">
         <v>11</v>
       </c>
@@ -1131,7 +1122,7 @@
       <c r="E13" s="12" t="n"/>
       <c r="F13" s="12" t="n"/>
       <c r="G13" s="12" t="n"/>
-      <c r="H13" s="47" t="s"/>
+      <c r="H13" s="58" t="s"/>
       <c r="I13" s="14" t="s">
         <v>12</v>
       </c>
@@ -1140,9 +1131,9 @@
       <c r="L13" s="12" t="n"/>
       <c r="M13" s="6" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="14" s="56" spans="1:13" thickBot="1">
+    <row customHeight="1" ht="20.1" r="14" s="55" spans="1:13">
       <c r="A14" s="11" t="n"/>
-      <c r="B14" s="47" t="s"/>
+      <c r="B14" s="58" t="s"/>
       <c r="C14" s="14" t="s">
         <v>13</v>
       </c>
@@ -1150,7 +1141,7 @@
       <c r="E14" s="12" t="n"/>
       <c r="F14" s="12" t="n"/>
       <c r="G14" s="12" t="n"/>
-      <c r="H14" s="47" t="s"/>
+      <c r="H14" s="58" t="s"/>
       <c r="I14" s="14" t="s">
         <v>14</v>
       </c>
@@ -1159,9 +1150,9 @@
       <c r="L14" s="12" t="n"/>
       <c r="M14" s="6" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="15" s="56" spans="1:13" thickBot="1">
+    <row customHeight="1" ht="20.1" r="15" s="55" spans="1:13">
       <c r="A15" s="11" t="n"/>
-      <c r="B15" s="47" t="s"/>
+      <c r="B15" s="58" t="s"/>
       <c r="C15" s="14" t="s">
         <v>15</v>
       </c>
@@ -1169,7 +1160,7 @@
       <c r="E15" s="12" t="n"/>
       <c r="F15" s="12" t="n"/>
       <c r="G15" s="12" t="n"/>
-      <c r="H15" s="47" t="s"/>
+      <c r="H15" s="58" t="s"/>
       <c r="I15" s="14" t="s">
         <v>16</v>
       </c>
@@ -1178,9 +1169,9 @@
       <c r="L15" s="12" t="n"/>
       <c r="M15" s="6" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="16" s="56" spans="1:13" thickBot="1">
+    <row customHeight="1" ht="20.1" r="16" s="55" spans="1:13">
       <c r="A16" s="11" t="n"/>
-      <c r="B16" s="47" t="s"/>
+      <c r="B16" s="58" t="s"/>
       <c r="C16" s="14" t="s">
         <v>17</v>
       </c>
@@ -1188,7 +1179,7 @@
       <c r="E16" s="12" t="n"/>
       <c r="F16" s="12" t="n"/>
       <c r="G16" s="12" t="n"/>
-      <c r="H16" s="47" t="s"/>
+      <c r="H16" s="58" t="s"/>
       <c r="I16" s="14" t="s">
         <v>18</v>
       </c>
@@ -1197,9 +1188,9 @@
       <c r="L16" s="12" t="n"/>
       <c r="M16" s="6" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="17" s="56" spans="1:13" thickBot="1">
+    <row customHeight="1" ht="20.1" r="17" s="55" spans="1:13">
       <c r="A17" s="11" t="n"/>
-      <c r="B17" s="47" t="s"/>
+      <c r="B17" s="58" t="s"/>
       <c r="C17" s="14" t="s">
         <v>19</v>
       </c>
@@ -1207,7 +1198,7 @@
       <c r="E17" s="12" t="n"/>
       <c r="F17" s="12" t="n"/>
       <c r="G17" s="12" t="n"/>
-      <c r="H17" s="47" t="s"/>
+      <c r="H17" s="58" t="s"/>
       <c r="I17" s="14" t="s">
         <v>20</v>
       </c>
@@ -1216,9 +1207,9 @@
       <c r="L17" s="12" t="n"/>
       <c r="M17" s="6" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="18" s="56" spans="1:13" thickBot="1">
+    <row customHeight="1" ht="20.1" r="18" s="55" spans="1:13">
       <c r="A18" s="11" t="n"/>
-      <c r="B18" s="47" t="s"/>
+      <c r="B18" s="58" t="s"/>
       <c r="C18" s="14" t="s">
         <v>21</v>
       </c>
@@ -1226,20 +1217,20 @@
       <c r="E18" s="12" t="n"/>
       <c r="F18" s="12" t="n"/>
       <c r="G18" s="12" t="n"/>
-      <c r="H18" s="47" t="s">
+      <c r="H18" s="58" t="s"/>
+      <c r="I18" s="15" t="s">
         <v>22</v>
-      </c>
-      <c r="I18" s="15" t="s">
-        <v>23</v>
       </c>
       <c r="J18" s="12" t="n"/>
       <c r="K18" s="12" t="n"/>
       <c r="L18" s="12" t="n"/>
       <c r="M18" s="6" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="19" s="56" spans="1:13" thickBot="1">
+    <row customHeight="1" ht="20.1" r="19" s="55" spans="1:13">
       <c r="A19" s="11" t="n"/>
-      <c r="B19" s="47" t="s"/>
+      <c r="B19" s="58" t="s">
+        <v>23</v>
+      </c>
       <c r="C19" s="13" t="s">
         <v>24</v>
       </c>
@@ -1247,82 +1238,82 @@
       <c r="E19" s="16" t="n"/>
       <c r="F19" s="16" t="n"/>
       <c r="G19" s="16" t="n"/>
-      <c r="H19" s="49" t="s"/>
+      <c r="H19" s="48" t="s"/>
       <c r="I19" s="16" t="n"/>
       <c r="J19" s="16" t="n"/>
       <c r="K19" s="16" t="n"/>
       <c r="L19" s="12" t="n"/>
       <c r="M19" s="6" t="n"/>
     </row>
-    <row customHeight="1" ht="3.95" r="20" s="56" spans="1:13" thickBot="1">
+    <row customHeight="1" ht="3.95" r="20" s="55" spans="1:13" thickBot="1">
       <c r="A20" s="7" t="n"/>
-      <c r="B20" s="50" t="s"/>
+      <c r="B20" s="49" t="s"/>
       <c r="C20" s="22" t="n"/>
       <c r="D20" s="22" t="n"/>
       <c r="E20" s="22" t="n"/>
       <c r="F20" s="22" t="n"/>
       <c r="G20" s="22" t="n"/>
-      <c r="H20" s="50" t="s"/>
+      <c r="H20" s="49" t="s"/>
       <c r="I20" s="22" t="n"/>
       <c r="J20" s="22" t="n"/>
       <c r="K20" s="22" t="n"/>
       <c r="L20" s="22" t="n"/>
       <c r="M20" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="3.95" r="21" s="56" spans="1:13">
+    <row customHeight="1" ht="3.95" r="21" s="55" spans="1:13">
       <c r="A21" s="3" t="n"/>
-      <c r="B21" s="51" t="s"/>
+      <c r="B21" s="50" t="s"/>
       <c r="C21" s="23" t="n"/>
       <c r="D21" s="23" t="n"/>
       <c r="E21" s="23" t="n"/>
       <c r="F21" s="23" t="n"/>
       <c r="G21" s="23" t="n"/>
-      <c r="H21" s="51" t="s"/>
+      <c r="H21" s="50" t="s"/>
       <c r="I21" s="23" t="n"/>
       <c r="J21" s="23" t="n"/>
       <c r="K21" s="23" t="n"/>
       <c r="L21" s="23" t="n"/>
       <c r="M21" s="5" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="22" s="56" spans="1:13">
+    <row customHeight="1" ht="15" r="22" s="55" spans="1:13">
       <c r="A22" s="11" t="n"/>
-      <c r="B22" s="52" t="s"/>
-      <c r="C22" s="12" t="n"/>
-      <c r="D22" s="10" t="s">
+      <c r="B22" s="51" t="s"/>
+      <c r="C22" s="56" t="n"/>
+      <c r="D22" s="57" t="s">
         <v>25</v>
       </c>
       <c r="E22" s="16" t="n">
         <v>8000</v>
       </c>
       <c r="F22" s="45" t="n">
-        <v>1235</v>
+        <v>78969</v>
       </c>
       <c r="G22" s="12" t="n"/>
-      <c r="H22" s="52" t="s"/>
+      <c r="H22" s="51" t="s"/>
       <c r="I22" s="12" t="n"/>
       <c r="J22" s="12" t="n"/>
       <c r="K22" s="12" t="n"/>
       <c r="L22" s="12" t="n"/>
       <c r="M22" s="6" t="n"/>
     </row>
-    <row customHeight="1" ht="3.95" r="23" s="56" spans="1:13">
+    <row customHeight="1" ht="3.95" r="23" s="55" spans="1:13">
       <c r="A23" s="18" t="n"/>
-      <c r="B23" s="53" t="s"/>
+      <c r="B23" s="52" t="s"/>
       <c r="C23" s="24" t="n"/>
       <c r="D23" s="24" t="n"/>
       <c r="E23" s="24" t="n"/>
       <c r="F23" s="24" t="n"/>
       <c r="G23" s="24" t="n"/>
-      <c r="H23" s="53" t="s"/>
+      <c r="H23" s="52" t="s"/>
       <c r="I23" s="24" t="n"/>
       <c r="J23" s="24" t="n"/>
       <c r="K23" s="24" t="n"/>
       <c r="L23" s="24" t="n"/>
       <c r="M23" s="19" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="24" s="56" spans="1:13" thickBot="1">
+    <row customHeight="1" ht="15" r="24" s="55" spans="1:13">
       <c r="A24" s="11" t="n"/>
-      <c r="B24" s="52" t="s"/>
+      <c r="B24" s="51" t="s"/>
       <c r="C24" s="12" t="s">
         <v>26</v>
       </c>
@@ -1330,16 +1321,16 @@
       <c r="E24" s="12" t="n"/>
       <c r="F24" s="12" t="n"/>
       <c r="G24" s="12" t="n"/>
-      <c r="H24" s="52" t="s"/>
+      <c r="H24" s="51" t="s"/>
       <c r="I24" s="12" t="n"/>
       <c r="J24" s="12" t="n"/>
       <c r="K24" s="12" t="n"/>
       <c r="L24" s="12" t="n"/>
       <c r="M24" s="6" t="n"/>
     </row>
-    <row customHeight="1" ht="15" r="25" s="56" spans="1:13" thickBot="1">
+    <row customHeight="1" ht="15" r="25" s="55" spans="1:13">
       <c r="A25" s="11" t="n"/>
-      <c r="B25" s="47" t="s"/>
+      <c r="B25" s="58" t="s"/>
       <c r="C25" s="12" t="s">
         <v>27</v>
       </c>
@@ -1347,7 +1338,7 @@
       <c r="E25" s="12" t="n"/>
       <c r="F25" s="12" t="n"/>
       <c r="G25" s="12" t="n"/>
-      <c r="H25" s="47" t="s"/>
+      <c r="H25" s="58" t="s"/>
       <c r="I25" s="12" t="s">
         <v>28</v>
       </c>
@@ -1356,9 +1347,9 @@
       <c r="L25" s="12" t="n"/>
       <c r="M25" s="6" t="n"/>
     </row>
-    <row customHeight="1" ht="15.75" r="26" s="56" spans="1:13" thickBot="1">
+    <row customHeight="1" ht="15.75" r="26" s="55" spans="1:13">
       <c r="A26" s="11" t="n"/>
-      <c r="B26" s="47" t="s"/>
+      <c r="B26" s="58" t="s"/>
       <c r="C26" s="12" t="s">
         <v>29</v>
       </c>
@@ -1366,7 +1357,7 @@
       <c r="E26" s="12" t="n"/>
       <c r="F26" s="12" t="n"/>
       <c r="G26" s="12" t="n"/>
-      <c r="H26" s="47" t="s"/>
+      <c r="H26" s="58" t="s"/>
       <c r="I26" s="12" t="s">
         <v>30</v>
       </c>
@@ -1375,9 +1366,9 @@
       <c r="L26" s="12" t="n"/>
       <c r="M26" s="6" t="n"/>
     </row>
-    <row customHeight="1" ht="15.75" r="27" s="56" spans="1:13" thickBot="1">
+    <row customHeight="1" ht="15.75" r="27" s="55" spans="1:13">
       <c r="A27" s="11" t="n"/>
-      <c r="B27" s="47" t="s"/>
+      <c r="B27" s="58" t="s"/>
       <c r="C27" s="12" t="s">
         <v>31</v>
       </c>
@@ -1385,7 +1376,7 @@
       <c r="E27" s="12" t="n"/>
       <c r="F27" s="12" t="n"/>
       <c r="G27" s="12" t="n"/>
-      <c r="H27" s="47" t="s"/>
+      <c r="H27" s="58" t="s"/>
       <c r="I27" s="12" t="s">
         <v>32</v>
       </c>
@@ -1394,9 +1385,9 @@
       <c r="L27" s="12" t="n"/>
       <c r="M27" s="6" t="n"/>
     </row>
-    <row customHeight="1" ht="15.75" r="28" s="56" spans="1:13" thickBot="1">
+    <row customHeight="1" ht="15.75" r="28" s="55" spans="1:13">
       <c r="A28" s="11" t="n"/>
-      <c r="B28" s="47" t="s"/>
+      <c r="B28" s="58" t="s"/>
       <c r="C28" s="12" t="s">
         <v>33</v>
       </c>
@@ -1404,7 +1395,7 @@
       <c r="E28" s="12" t="n"/>
       <c r="F28" s="12" t="n"/>
       <c r="G28" s="12" t="n"/>
-      <c r="H28" s="47" t="s"/>
+      <c r="H28" s="58" t="s"/>
       <c r="I28" s="12" t="s">
         <v>34</v>
       </c>
@@ -1413,9 +1404,9 @@
       <c r="L28" s="12" t="n"/>
       <c r="M28" s="6" t="n"/>
     </row>
-    <row customHeight="1" ht="15.75" r="29" s="56" spans="1:13" thickBot="1">
+    <row customHeight="1" ht="15.75" r="29" s="55" spans="1:13">
       <c r="A29" s="11" t="n"/>
-      <c r="B29" s="47" t="s"/>
+      <c r="B29" s="58" t="s"/>
       <c r="C29" s="13" t="s">
         <v>24</v>
       </c>
@@ -1423,63 +1414,63 @@
       <c r="E29" s="16" t="n"/>
       <c r="F29" s="16" t="n"/>
       <c r="G29" s="16" t="n"/>
-      <c r="H29" s="49" t="s"/>
+      <c r="H29" s="48" t="s"/>
       <c r="I29" s="16" t="n"/>
       <c r="J29" s="16" t="n"/>
       <c r="K29" s="16" t="n"/>
       <c r="L29" s="12" t="n"/>
       <c r="M29" s="6" t="n"/>
     </row>
-    <row customHeight="1" ht="3.95" r="30" s="56" spans="1:13">
+    <row customHeight="1" ht="3.95" r="30" s="55" spans="1:13">
       <c r="A30" s="20" t="n"/>
-      <c r="B30" s="49" t="s"/>
+      <c r="B30" s="48" t="s"/>
       <c r="C30" s="16" t="n"/>
       <c r="D30" s="16" t="n"/>
       <c r="E30" s="16" t="n"/>
       <c r="F30" s="16" t="n"/>
       <c r="G30" s="16" t="n"/>
-      <c r="H30" s="49" t="s"/>
+      <c r="H30" s="48" t="s"/>
       <c r="I30" s="16" t="n"/>
       <c r="J30" s="16" t="n"/>
       <c r="K30" s="16" t="n"/>
       <c r="L30" s="16" t="n"/>
       <c r="M30" s="21" t="n"/>
     </row>
-    <row customHeight="1" ht="3.95" r="31" s="56" spans="1:13">
+    <row customHeight="1" ht="3.95" r="31" s="55" spans="1:13">
       <c r="A31" s="11" t="n"/>
-      <c r="B31" s="52" t="s"/>
+      <c r="B31" s="51" t="s"/>
       <c r="C31" s="12" t="n"/>
       <c r="D31" s="12" t="n"/>
       <c r="E31" s="12" t="n"/>
       <c r="F31" s="12" t="n"/>
       <c r="G31" s="12" t="n"/>
-      <c r="H31" s="52" t="s"/>
+      <c r="H31" s="51" t="s"/>
       <c r="I31" s="12" t="n"/>
       <c r="J31" s="12" t="n"/>
       <c r="K31" s="12" t="n"/>
       <c r="L31" s="12" t="n"/>
       <c r="M31" s="6" t="n"/>
     </row>
-    <row customHeight="1" ht="15.75" r="32" s="56" spans="1:13" thickBot="1">
+    <row customHeight="1" ht="15.75" r="32" s="55" spans="1:13">
       <c r="A32" s="11" t="n"/>
-      <c r="B32" s="52" t="s"/>
-      <c r="C32" s="12" t="s">
+      <c r="B32" s="51" t="s"/>
+      <c r="C32" s="56" t="s">
         <v>35</v>
       </c>
       <c r="D32" s="12" t="n"/>
       <c r="E32" s="12" t="n"/>
       <c r="F32" s="12" t="n"/>
       <c r="G32" s="12" t="n"/>
-      <c r="H32" s="52" t="s"/>
+      <c r="H32" s="51" t="s"/>
       <c r="I32" s="12" t="n"/>
       <c r="J32" s="12" t="n"/>
       <c r="K32" s="12" t="n"/>
       <c r="L32" s="12" t="n"/>
       <c r="M32" s="6" t="n"/>
     </row>
-    <row customHeight="1" ht="15.75" r="33" s="56" spans="1:13" thickBot="1">
+    <row customHeight="1" ht="15.75" r="33" s="55" spans="1:13">
       <c r="A33" s="11" t="n"/>
-      <c r="B33" s="47" t="s"/>
+      <c r="B33" s="58" t="s"/>
       <c r="C33" s="12" t="s">
         <v>36</v>
       </c>
@@ -1487,9 +1478,7 @@
       <c r="E33" s="12" t="n"/>
       <c r="F33" s="12" t="n"/>
       <c r="G33" s="12" t="n"/>
-      <c r="H33" s="47" t="s">
-        <v>22</v>
-      </c>
+      <c r="H33" s="58" t="s"/>
       <c r="I33" s="14" t="s">
         <v>37</v>
       </c>
@@ -1498,9 +1487,11 @@
       <c r="L33" s="12" t="n"/>
       <c r="M33" s="6" t="n"/>
     </row>
-    <row customHeight="1" ht="15.75" r="34" s="56" spans="1:13" thickBot="1">
+    <row customHeight="1" ht="15.75" r="34" s="55" spans="1:13">
       <c r="A34" s="11" t="n"/>
-      <c r="B34" s="47" t="s"/>
+      <c r="B34" s="58" t="s">
+        <v>23</v>
+      </c>
       <c r="C34" s="13" t="s">
         <v>24</v>
       </c>
@@ -1515,7 +1506,7 @@
       <c r="L34" s="12" t="n"/>
       <c r="M34" s="6" t="n"/>
     </row>
-    <row customHeight="1" ht="3.95" r="35" s="56" spans="1:13" thickBot="1">
+    <row customHeight="1" ht="3.95" r="35" s="55" spans="1:13" thickBot="1">
       <c r="A35" s="7" t="n"/>
       <c r="B35" s="22" t="n"/>
       <c r="C35" s="22" t="n"/>
@@ -1530,7 +1521,7 @@
       <c r="L35" s="22" t="n"/>
       <c r="M35" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="3.95" r="36" s="56" spans="1:13">
+    <row customHeight="1" ht="3.95" r="36" s="55" spans="1:13">
       <c r="B36" s="12" t="n"/>
       <c r="C36" s="12" t="n"/>
       <c r="D36" s="12" t="n"/>
@@ -1544,7 +1535,7 @@
       <c r="L36" s="12" t="n"/>
     </row>
     <row r="37" spans="1:13">
-      <c r="C37" s="12" t="s">
+      <c r="C37" s="56" t="s">
         <v>38</v>
       </c>
       <c r="D37" s="12" t="n"/>
@@ -1656,8 +1647,8 @@
       <c r="K44" s="27" t="n"/>
       <c r="L44" s="34" t="n"/>
     </row>
-    <row customHeight="1" ht="15.75" r="45" s="56" spans="1:13" thickBot="1"/>
-    <row customHeight="1" ht="3.95" r="46" s="56" spans="1:13">
+    <row customHeight="1" ht="15.75" r="45" s="55" spans="1:13" thickBot="1"/>
+    <row customHeight="1" ht="3.95" r="46" s="55" spans="1:13">
       <c r="A46" s="3" t="n"/>
       <c r="B46" s="4" t="n"/>
       <c r="C46" s="4" t="n"/>
@@ -1685,7 +1676,7 @@
       <c r="K47" s="16" t="n"/>
       <c r="M47" s="6" t="n"/>
     </row>
-    <row customHeight="1" ht="3.95" r="48" s="56" spans="1:13" thickBot="1">
+    <row customHeight="1" ht="3.95" r="48" s="55" spans="1:13" thickBot="1">
       <c r="A48" s="7" t="n"/>
       <c r="B48" s="8" t="n"/>
       <c r="C48" s="8" t="n"/>
@@ -1700,7 +1691,7 @@
       <c r="L48" s="8" t="n"/>
       <c r="M48" s="9" t="n"/>
     </row>
-    <row customHeight="1" ht="3.95" r="50" s="56" spans="1:13">
+    <row customHeight="1" ht="3.95" r="50" s="55" spans="1:13">
       <c r="A50" s="36" t="n"/>
       <c r="B50" s="37" t="n"/>
       <c r="C50" s="37" t="n"/>
@@ -1717,7 +1708,7 @@
     </row>
     <row r="51" spans="1:13">
       <c r="A51" s="39" t="n"/>
-      <c r="C51" s="48" t="s">
+      <c r="C51" s="47" t="s">
         <v>44</v>
       </c>
       <c r="M51" s="40" t="n"/>
@@ -1727,8 +1718,8 @@
       <c r="C52" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="D52" s="55" t="n">
-        <v>123456789</v>
+      <c r="D52" s="54" t="n">
+        <v>1</v>
       </c>
       <c r="M52" s="40" t="n"/>
     </row>

</xml_diff>

<commit_message>
find type_eq and file eq
</commit_message>
<xml_diff>
--- a/f2-02-04-5.xlsx
+++ b/f2-02-04-5.xlsx
@@ -22,13 +22,13 @@
     <t>дата:</t>
   </si>
   <si>
-    <t>16/01/2018</t>
+    <t>23/01/2018</t>
   </si>
   <si>
     <t>час:</t>
   </si>
   <si>
-    <t>20:42</t>
+    <t>23:13</t>
   </si>
   <si>
     <t>Автор повідомлення:</t>
@@ -1286,7 +1286,7 @@
         <v>8000</v>
       </c>
       <c r="F22" s="45" t="n">
-        <v>1236</v>
+        <v>1111</v>
       </c>
       <c r="G22" s="12" t="n"/>
       <c r="H22" s="51" t="s"/>
@@ -1330,7 +1330,9 @@
     </row>
     <row customHeight="1" ht="15" r="25" s="55" spans="1:13">
       <c r="A25" s="11" t="n"/>
-      <c r="B25" s="58" t="s"/>
+      <c r="B25" s="58" t="s">
+        <v>7</v>
+      </c>
       <c r="C25" s="12" t="s">
         <v>27</v>
       </c>

</xml_diff>

<commit_message>
add check counter number by rising
</commit_message>
<xml_diff>
--- a/f2-02-04-5.xlsx
+++ b/f2-02-04-5.xlsx
@@ -22,13 +22,13 @@
     <t>дата:</t>
   </si>
   <si>
-    <t>31/01/2018</t>
+    <t>06/02/2018</t>
   </si>
   <si>
     <t>час:</t>
   </si>
   <si>
-    <t>22:26</t>
+    <t>23:40</t>
   </si>
   <si>
     <t>Автор повідомлення:</t>
@@ -58,6 +58,9 @@
     <t>Пошкодження контакту або його деформація</t>
   </si>
   <si>
+    <t>X</t>
+  </si>
+  <si>
     <t>Не відповідне термоусадження</t>
   </si>
   <si>
@@ -83,9 +86,6 @@
   </si>
   <si>
     <t>Обладнання не вмикається / не продукує виріб</t>
-  </si>
-  <si>
-    <t>X</t>
   </si>
   <si>
     <t>Інше:</t>
@@ -1141,9 +1141,11 @@
       <c r="E14" s="12" t="n"/>
       <c r="F14" s="12" t="n"/>
       <c r="G14" s="12" t="n"/>
-      <c r="H14" s="58" t="s"/>
+      <c r="H14" s="58" t="s">
+        <v>14</v>
+      </c>
       <c r="I14" s="14" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="J14" s="12" t="n"/>
       <c r="K14" s="12" t="n"/>
@@ -1154,7 +1156,7 @@
       <c r="A15" s="11" t="n"/>
       <c r="B15" s="58" t="s"/>
       <c r="C15" s="14" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D15" s="12" t="n"/>
       <c r="E15" s="12" t="n"/>
@@ -1162,7 +1164,7 @@
       <c r="G15" s="12" t="n"/>
       <c r="H15" s="58" t="s"/>
       <c r="I15" s="14" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J15" s="12" t="n"/>
       <c r="K15" s="12" t="n"/>
@@ -1173,7 +1175,7 @@
       <c r="A16" s="11" t="n"/>
       <c r="B16" s="58" t="s"/>
       <c r="C16" s="14" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D16" s="12" t="n"/>
       <c r="E16" s="12" t="n"/>
@@ -1181,7 +1183,7 @@
       <c r="G16" s="12" t="n"/>
       <c r="H16" s="58" t="s"/>
       <c r="I16" s="14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J16" s="12" t="n"/>
       <c r="K16" s="12" t="n"/>
@@ -1192,7 +1194,7 @@
       <c r="A17" s="11" t="n"/>
       <c r="B17" s="58" t="s"/>
       <c r="C17" s="14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D17" s="12" t="n"/>
       <c r="E17" s="12" t="n"/>
@@ -1200,7 +1202,7 @@
       <c r="G17" s="12" t="n"/>
       <c r="H17" s="58" t="s"/>
       <c r="I17" s="14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="J17" s="12" t="n"/>
       <c r="K17" s="12" t="n"/>
@@ -1211,7 +1213,7 @@
       <c r="A18" s="11" t="n"/>
       <c r="B18" s="58" t="s"/>
       <c r="C18" s="14" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D18" s="12" t="n"/>
       <c r="E18" s="12" t="n"/>
@@ -1219,7 +1221,7 @@
       <c r="G18" s="12" t="n"/>
       <c r="H18" s="58" t="s"/>
       <c r="I18" s="15" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="J18" s="12" t="n"/>
       <c r="K18" s="12" t="n"/>
@@ -1228,9 +1230,7 @@
     </row>
     <row customHeight="1" ht="20.1" r="19" s="55" spans="1:13">
       <c r="A19" s="11" t="n"/>
-      <c r="B19" s="58" t="s">
-        <v>23</v>
-      </c>
+      <c r="B19" s="58" t="s"/>
       <c r="C19" s="13" t="s">
         <v>24</v>
       </c>
@@ -1350,7 +1350,7 @@
     <row customHeight="1" ht="15.75" r="26" s="55" spans="1:13">
       <c r="A26" s="11" t="n"/>
       <c r="B26" s="58" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="C26" s="12" t="s">
         <v>29</v>
@@ -1473,7 +1473,7 @@
     <row customHeight="1" ht="15.75" r="33" s="55" spans="1:13">
       <c r="A33" s="11" t="n"/>
       <c r="B33" s="58" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="C33" s="12" t="s">
         <v>36</v>
@@ -1721,7 +1721,7 @@
         <v>45</v>
       </c>
       <c r="D52" s="54" t="n">
-        <v>123456</v>
+        <v>35</v>
       </c>
       <c r="M52" s="40" t="n"/>
     </row>

</xml_diff>